<commit_message>
[HF-36][Zhen Tang]fix: fix the baby report header
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/Healthy-Future-Report-Baby.xlsx
+++ b/src/main/resources/static/excel/Healthy-Future-Report-Baby.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ztang/workspace/unc/src/visit-link-service/src/main/resources/static/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5E2DB3-0B59-B847-82BE-7B8DC8D5FBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C8A29C-7152-DC48-8943-143A3234554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="3640" windowWidth="22360" windowHeight="9560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5900" yWindow="4020" windowWidth="29400" windowHeight="14980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baby Roster" sheetId="1" r:id="rId1"/>
@@ -67,9 +67,6 @@
     <t>Birth_Date</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>Caregiver V_Wechat</t>
   </si>
   <si>
-    <t>Remark (备注信息）</t>
-  </si>
-  <si>
     <t>Baby’s EDC</t>
   </si>
   <si>
@@ -188,6 +182,12 @@
   </si>
   <si>
     <t>reason_archive</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -594,125 +594,125 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>